<commit_message>
* Fixed feather bugs - Feather debugging functions added ! Not working feather - Updated upload scripts - Updated calculations for selected fabrics
</commit_message>
<xml_diff>
--- a/Documents/Blueprints/calculations.xlsx
+++ b/Documents/Blueprints/calculations.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
   <si>
     <t>Баллон</t>
   </si>
@@ -163,6 +163,27 @@
   </si>
   <si>
     <t>50-60</t>
+  </si>
+  <si>
+    <t>красненькая ткань</t>
+  </si>
+  <si>
+    <t>Размеры</t>
+  </si>
+  <si>
+    <t>Итоговый размер</t>
+  </si>
+  <si>
+    <t>Выкройка</t>
+  </si>
+  <si>
+    <t>Площадь ткани</t>
+  </si>
+  <si>
+    <t>м</t>
+  </si>
+  <si>
+    <t>м2</t>
   </si>
 </sst>
 </file>
@@ -235,7 +256,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -246,56 +267,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -578,7 +550,7 @@
   <dimension ref="A2:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,14 +578,14 @@
       </c>
       <c r="B3">
         <f>Баллон!E19</f>
-        <v>723.51359999999988</v>
+        <v>405.30160000000006</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D12" si="0">C3*B3</f>
-        <v>723.51359999999988</v>
+        <v>405.30160000000006</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -766,7 +738,7 @@
       </c>
       <c r="D15">
         <f>SUM(D3:D14)</f>
-        <v>839.11359999999991</v>
+        <v>520.90160000000014</v>
       </c>
       <c r="E15" t="s">
         <v>34</v>
@@ -778,7 +750,7 @@
       </c>
       <c r="D16">
         <f>Баллон!E14*1000</f>
-        <v>1016.1625996799996</v>
+        <v>782.70394686000009</v>
       </c>
       <c r="E16" t="s">
         <v>34</v>
@@ -787,12 +759,12 @@
     <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
         <f>D16-D15</f>
-        <v>177.04899967999972</v>
+        <v>261.80234685999994</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D20">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -803,10 +775,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -840,7 +812,7 @@
       </c>
       <c r="E2">
         <f>C2/E12</f>
-        <v>2.3868</v>
+        <v>2.1879000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -857,7 +829,7 @@
       </c>
       <c r="E3">
         <f>C3/E12</f>
-        <v>2.9164320000000004</v>
+        <v>2.6733960000000003</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -873,7 +845,7 @@
       </c>
       <c r="E4">
         <f>C4/E12</f>
-        <v>0.46439999999999998</v>
+        <v>0.42570000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -889,7 +861,7 @@
       </c>
       <c r="E5" s="4">
         <f>C5/E12</f>
-        <v>2.01756</v>
+        <v>1.8494300000000001</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -905,7 +877,7 @@
       </c>
       <c r="E6">
         <f>C6/E12</f>
-        <v>0.91776000000000002</v>
+        <v>0.84128000000000003</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -932,7 +904,7 @@
       </c>
       <c r="E8">
         <f>C8/(E12^2)</f>
-        <v>4.8234239999999993</v>
+        <v>4.0530160000000004</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -959,7 +931,7 @@
       </c>
       <c r="E10">
         <f>C10/(E12^3)</f>
-        <v>0.84680216639999983</v>
+        <v>0.65225328905000013</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -968,10 +940,10 @@
       </c>
       <c r="E12" s="1">
         <f>1/F12</f>
-        <v>0.83333333333333337</v>
+        <v>0.90909090909090906</v>
       </c>
       <c r="F12">
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -989,7 +961,7 @@
       </c>
       <c r="E14">
         <f>1.2*E10</f>
-        <v>1.0161625996799997</v>
+        <v>0.78270394686000011</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1024,14 +996,14 @@
         <v>30</v>
       </c>
       <c r="B17">
-        <v>1.4999999999999999E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="C17" t="s">
         <v>32</v>
       </c>
       <c r="E17">
         <f>B17*1000000</f>
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="F17" t="s">
         <v>33</v>
@@ -1063,11 +1035,11 @@
       </c>
       <c r="C19">
         <f>E17*E16*C8</f>
-        <v>502.44</v>
+        <v>334.96000000000004</v>
       </c>
       <c r="E19">
         <f>E17*E16*E8</f>
-        <v>723.51359999999988</v>
+        <v>405.30160000000006</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1081,15 +1053,98 @@
         <v>44</v>
       </c>
     </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>46</v>
+      </c>
+      <c r="J21">
+        <v>100</v>
+      </c>
+    </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E25" s="3">
         <f>Sheet1!D16-Sheet1!D15</f>
-        <v>177.04899967999972</v>
+        <v>261.80234685999994</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28">
+        <v>1407.21</v>
+      </c>
+      <c r="C28">
+        <v>174.93</v>
+      </c>
+      <c r="D28">
+        <v>79.84</v>
+      </c>
+      <c r="E28">
+        <v>82.38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29">
+        <f>(E2*1000)/(B28+D28+E28)</f>
+        <v>1.3940730073975907</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30">
+        <f>B28*B29</f>
+        <v>1961.7534767399636</v>
+      </c>
+      <c r="C30">
+        <f>C28*B29</f>
+        <v>243.86519118406054</v>
+      </c>
+      <c r="D30">
+        <f>D28*B29</f>
+        <v>111.30278891062365</v>
+      </c>
+      <c r="E30">
+        <f>E28*B29</f>
+        <v>114.84373434941351</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32">
+        <f>B30</f>
+        <v>1961.7534767399636</v>
+      </c>
+      <c r="C32">
+        <f>12*C30</f>
+        <v>2926.3822942087263</v>
+      </c>
+      <c r="D32" t="s">
+        <v>51</v>
+      </c>
+      <c r="F32">
+        <f>B32/1000 * C32/1000</f>
+        <v>5.7408406399342402</v>
+      </c>
+      <c r="G32" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>